<commit_message>
Added courier frontend part to handle shipment assignments
</commit_message>
<xml_diff>
--- a/Persistence/Database/test_data/Shipments.xlsx
+++ b/Persistence/Database/test_data/Shipments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vieva\Desktop\PSK\komandinis\shipping-service\Persistence\Database\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hardas\projects\shipping-service\Persistence\Database\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F9D389-DF4B-461E-9FCA-3F52830B4152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BC29A6-B693-446C-AE24-78E70CD41573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -116,6 +116,24 @@
   </si>
   <si>
     <t>Greetings. Congrats for passing the exam. The driving license if coming to you. Drive safely.</t>
+  </si>
+  <si>
+    <t>Sulčių pakelis</t>
+  </si>
+  <si>
+    <t>Renki visokį šlamštą, gal panaudosi</t>
+  </si>
+  <si>
+    <t>megztinis</t>
+  </si>
+  <si>
+    <t>kad nesušaltum</t>
+  </si>
+  <si>
+    <t>kačiukas</t>
+  </si>
+  <si>
+    <t>Gimtadienio dovana</t>
   </si>
 </sst>
 </file>
@@ -968,22 +986,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="46.88671875" customWidth="1"/>
-    <col min="4" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" customWidth="1"/>
-    <col min="7" max="8" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.3125" customWidth="1"/>
+    <col min="3" max="3" width="46.89453125" customWidth="1"/>
+    <col min="4" max="5" width="12.68359375" customWidth="1"/>
+    <col min="6" max="6" width="22.1015625" customWidth="1"/>
+    <col min="7" max="8" width="22.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="79.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1035,7 +1053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="83.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1059,7 +1077,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1085,7 +1103,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1107,7 +1125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="85.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1131,7 +1149,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="92.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1157,7 +1175,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1183,7 +1201,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="104.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1207,7 +1225,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="52.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1233,7 +1251,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1257,6 +1275,75 @@
       </c>
       <c r="H11" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="1">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>5</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>